<commit_message>
Se modifica Excel Rendimiento
</commit_message>
<xml_diff>
--- a/Analisis de rendimiento.xlsx
+++ b/Analisis de rendimiento.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17329"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mariano.e.laurenti\Documents\GitHub\Matriz-VectorMath\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nicolás\Desktop\Programacion Avanzada\TPS\Matriz-VectorMath\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4455"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15348" windowHeight="4452"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -62,7 +62,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -125,29 +125,15 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
@@ -168,9 +154,9 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="es-ES"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -206,6 +192,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -230,7 +217,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="es-AR"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -283,10 +270,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$7</c:f>
+              <c:f>Sheet1!$A$2:$A$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>10</c:v>
                 </c:pt>
@@ -305,15 +292,18 @@
                 <c:pt idx="5">
                   <c:v>1000</c:v>
                 </c:pt>
+                <c:pt idx="6">
+                  <c:v>2000</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$7</c:f>
+              <c:f>Sheet1!$B$2:$B$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>39</c:v>
                 </c:pt>
@@ -332,11 +322,14 @@
                 <c:pt idx="5">
                   <c:v>20890</c:v>
                 </c:pt>
+                <c:pt idx="6">
+                  <c:v>26514</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-1839-4621-9264-A8B8E811C78A}"/>
             </c:ext>
@@ -350,11 +343,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="418323120"/>
-        <c:axId val="418322792"/>
+        <c:axId val="153333312"/>
+        <c:axId val="153333704"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="418323120"/>
+        <c:axId val="153333312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -400,6 +393,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -424,7 +418,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="es-AR"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -434,8 +428,9 @@
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
-          <a:ln>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
             <a:noFill/>
+            <a:round/>
           </a:ln>
           <a:effectLst/>
         </c:spPr>
@@ -455,15 +450,15 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-AR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="418322792"/>
+        <c:crossAx val="153333704"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="418322792"/>
+        <c:axId val="153333704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -509,6 +504,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -533,7 +529,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="es-AR"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -569,10 +565,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-AR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="418323120"/>
+        <c:crossAx val="153333312"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -613,7 +609,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="es-AR"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1222,7 +1218,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C74A11AD-B747-4EA5-960D-9F6D0927FA16}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{C74A11AD-B747-4EA5-960D-9F6D0927FA16}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1543,28 +1539,28 @@
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="5" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="3">
         <v>10</v>
       </c>
@@ -1576,7 +1572,7 @@
         <v>3.9E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="3">
         <v>20</v>
       </c>
@@ -1588,7 +1584,7 @@
         <v>7.0000000000000007E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="3">
         <v>50</v>
       </c>
@@ -1600,7 +1596,7 @@
         <v>0.13</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="3">
         <v>100</v>
       </c>
@@ -1612,7 +1608,7 @@
         <v>0.33100000000000002</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="3">
         <v>500</v>
       </c>
@@ -1624,25 +1620,33 @@
         <v>2.6779999999999999</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="4">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" s="3">
         <v>1000</v>
       </c>
-      <c r="B7" s="2">
+      <c r="B7" s="1">
         <v>20890</v>
       </c>
-      <c r="C7" s="2">
+      <c r="C7" s="1">
         <f t="shared" si="0"/>
         <v>20.89</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8">
+    <row r="8" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="2">
         <v>2000</v>
+      </c>
+      <c r="B8" s="2">
+        <v>26514</v>
+      </c>
+      <c r="C8" s="2">
+        <f>B8/1000</f>
+        <v>26.513999999999999</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>